<commit_message>
change due to comments
</commit_message>
<xml_diff>
--- a/data/wang2020fecal/A data.xlsx
+++ b/data/wang2020fecal/A data.xlsx
@@ -27,12 +27,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="14">
   <si>
     <t>patients</t>
   </si>
   <si>
     <t>days</t>
+  </si>
+  <si>
+    <t>ctvalue</t>
   </si>
   <si>
     <t>A</t>
@@ -1216,8 +1219,8 @@
   <sheetPr/>
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="2"/>
@@ -1226,17 +1229,20 @@
     <col min="3" max="3" width="12.9230769230769"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1">
         <v>9.95433789954337</v>
@@ -1247,7 +1253,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>13.9497716894977</v>
@@ -1258,7 +1264,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>18.1050228310502</v>
@@ -1269,7 +1275,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>20.1826484018264</v>
@@ -1280,7 +1286,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>15.0684931506849</v>
@@ -1291,7 +1297,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>19.2237442922374</v>
@@ -1302,7 +1308,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>21.9406392694063</v>
@@ -1313,18 +1319,18 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B9">
         <v>25.1369863013698</v>
       </c>
       <c r="C9">
-        <v>39.8958333333333</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B10">
         <v>18.9041095890411</v>
@@ -1335,7 +1341,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B11">
         <v>30.0913242009132</v>
@@ -1346,7 +1352,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B12">
         <v>32.1689497716895</v>
@@ -1357,7 +1363,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B13">
         <v>34.0867579908675</v>
@@ -1368,7 +1374,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B14">
         <v>36.324200913242</v>
@@ -1379,7 +1385,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B15">
         <v>8.03652968036529</v>
@@ -1390,7 +1396,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B16">
         <v>16.0273972602739</v>
@@ -1401,7 +1407,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B17">
         <v>19.8630136986301</v>
@@ -1412,7 +1418,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B18">
         <v>14.9086757990867</v>
@@ -1423,7 +1429,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B19">
         <v>18.1050228310502</v>
@@ -1434,7 +1440,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B20">
         <v>22.2602739726027</v>
@@ -1445,7 +1451,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B21">
         <v>28.3333333333333</v>
@@ -1456,7 +1462,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B22">
         <v>17.945205479452</v>
@@ -1467,7 +1473,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B23">
         <v>20.0228310502283</v>
@@ -1478,7 +1484,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B24">
         <v>24.337899543379</v>
@@ -1489,7 +1495,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B25">
         <v>12.8310502283105</v>
@@ -1500,7 +1506,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B26">
         <v>16.986301369863</v>
@@ -1511,7 +1517,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B27">
         <v>19.0639269406392</v>
@@ -1522,7 +1528,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B28">
         <v>24.9771689497716</v>
@@ -1533,7 +1539,7 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B29">
         <v>32.1689497716895</v>
@@ -1544,7 +1550,7 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B30">
         <v>34.0867579908675</v>
@@ -1555,7 +1561,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B31">
         <v>36.8036529680365</v>
@@ -1566,7 +1572,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B32">
         <v>38.0821917808219</v>
@@ -1577,7 +1583,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B33">
         <v>40.1598173515981</v>
@@ -1588,7 +1594,7 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B34">
         <v>40.958904109589</v>
@@ -1599,7 +1605,7 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B35">
         <v>44.1552511415525</v>
@@ -1610,7 +1616,7 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B36">
         <v>14.9086757990867</v>
@@ -1621,7 +1627,7 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B37">
         <v>16.986301369863</v>
@@ -1632,7 +1638,7 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B38">
         <v>18.9041095890411</v>
@@ -1643,7 +1649,7 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B39">
         <v>22.8995433789954</v>
@@ -1654,7 +1660,7 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B40">
         <v>28.972602739726</v>
@@ -1665,7 +1671,7 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B41">
         <v>31.0502283105022</v>
@@ -1676,7 +1682,7 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B42">
         <v>35.0456621004566</v>
@@ -1687,7 +1693,7 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B43">
         <v>36.0045662100456</v>
@@ -1698,7 +1704,7 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B44">
         <v>37.9223744292237</v>
@@ -1709,7 +1715,7 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B45">
         <v>39.0410958904109</v>
@@ -1720,7 +1726,7 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B46">
         <v>41.1187214611872</v>
@@ -1731,7 +1737,7 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B47">
         <v>42.2374429223744</v>
@@ -1742,7 +1748,7 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B48">
         <v>44.1552511415525</v>
@@ -1753,7 +1759,7 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B49">
         <v>46.2328767123287</v>
@@ -1764,7 +1770,7 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B50">
         <v>48.9497716894977</v>
@@ -1775,7 +1781,7 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B51">
         <v>50.0684931506849</v>
@@ -1786,7 +1792,7 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B52">
         <v>20.8219178082191</v>
@@ -1797,7 +1803,7 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B53">
         <v>23.8584474885844</v>
@@ -1808,7 +1814,7 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B54">
         <v>27.0547945205479</v>
@@ -1819,7 +1825,7 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B55">
         <v>29.1324200913242</v>
@@ -1830,7 +1836,7 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B56">
         <v>16.6666666666666</v>
@@ -1841,7 +1847,7 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B57">
         <v>24.0182648401826</v>

</xml_diff>

<commit_message>
change rounding method again
</commit_message>
<xml_diff>
--- a/data/wang2020fecal/A data.xlsx
+++ b/data/wang2020fecal/A data.xlsx
@@ -1219,8 +1219,8 @@
   <sheetPr/>
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="2"/>
@@ -1311,7 +1311,7 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>21.9406392694063</v>
+        <v>22.0406392694063</v>
       </c>
       <c r="C8">
         <v>27.8125</v>

</xml_diff>